<commit_message>
default value for xlsx
</commit_message>
<xml_diff>
--- a/docs/excel/TCar.xlsx
+++ b/docs/excel/TCar.xlsx
@@ -822,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1003,9 +1003,8 @@
       <c r="C5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="e">
-        <f>INT(P5*#REF!)</f>
-        <v>#REF!</v>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" t="s">
@@ -1014,6 +1013,27 @@
       <c r="G5" t="s">
         <v>24</v>
       </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
       <c r="O5">
         <v>0.2</v>
       </c>
@@ -1034,9 +1054,8 @@
       <c r="C6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="e">
-        <f>INT(P6*#REF!)</f>
-        <v>#REF!</v>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" t="s">
@@ -1045,6 +1064,27 @@
       <c r="G6" t="s">
         <v>28</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
       <c r="O6">
         <v>0.4</v>
       </c>
@@ -1065,9 +1105,8 @@
       <c r="C7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="e">
-        <f>INT(P7*#REF!)</f>
-        <v>#REF!</v>
+      <c r="D7">
+        <v>0</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" t="s">
@@ -1076,6 +1115,27 @@
       <c r="G7" t="s">
         <v>32</v>
       </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
       <c r="O7">
         <v>0.6</v>
       </c>
@@ -1096,9 +1156,8 @@
       <c r="C8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="e">
-        <f>INT(P8*#REF!)</f>
-        <v>#REF!</v>
+      <c r="D8">
+        <v>0</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" t="s">
@@ -1107,6 +1166,27 @@
       <c r="G8" t="s">
         <v>36</v>
       </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
       <c r="O8">
         <v>0.8</v>
       </c>
@@ -1127,9 +1207,8 @@
       <c r="C9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="e">
-        <f>INT(P9*#REF!)</f>
-        <v>#REF!</v>
+      <c r="D9">
+        <v>0</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" t="s">
@@ -1138,6 +1217,27 @@
       <c r="G9" t="s">
         <v>40</v>
       </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
       <c r="O9">
         <v>1</v>
       </c>
@@ -1158,9 +1258,8 @@
       <c r="C10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D10" t="e">
-        <f>INT(P10*#REF!)</f>
-        <v>#REF!</v>
+      <c r="D10">
+        <v>0</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" t="s">
@@ -1169,6 +1268,27 @@
       <c r="G10" t="s">
         <v>44</v>
       </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
       <c r="O10">
         <v>1.2</v>
       </c>
@@ -1189,9 +1309,8 @@
       <c r="C11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="e">
-        <f>INT(P11*#REF!)</f>
-        <v>#REF!</v>
+      <c r="D11">
+        <v>0</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" t="s">
@@ -1200,6 +1319,27 @@
       <c r="G11" t="s">
         <v>48</v>
       </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
       <c r="O11">
         <v>1.4</v>
       </c>
@@ -1220,9 +1360,8 @@
       <c r="C12" s="9">
         <v>911</v>
       </c>
-      <c r="D12" t="e">
-        <f>INT(P12*#REF!)</f>
-        <v>#REF!</v>
+      <c r="D12">
+        <v>0</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" t="s">
@@ -1231,6 +1370,27 @@
       <c r="G12" t="s">
         <v>51</v>
       </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
       <c r="O12">
         <v>1.6</v>
       </c>
@@ -1251,9 +1411,8 @@
       <c r="C13" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D13" t="e">
-        <f>INT(P13*#REF!)</f>
-        <v>#REF!</v>
+      <c r="D13">
+        <v>0</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" t="s">
@@ -1262,6 +1421,27 @@
       <c r="G13" t="s">
         <v>54</v>
       </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
       <c r="O13">
         <v>1.8</v>
       </c>
@@ -1282,9 +1462,8 @@
       <c r="C14" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="e">
-        <f>INT(P14*#REF!)</f>
-        <v>#REF!</v>
+      <c r="D14">
+        <v>0</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" t="s">
@@ -1292,6 +1471,27 @@
       </c>
       <c r="G14" t="s">
         <v>58</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
       </c>
       <c r="O14">
         <v>2</v>

</xml_diff>

<commit_message>
new car config xlsx
</commit_message>
<xml_diff>
--- a/docs/excel/TCar.xlsx
+++ b/docs/excel/TCar.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13650" tabRatio="204"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13650" tabRatio="204"/>
   </bookViews>
   <sheets>
     <sheet name="TCar" sheetId="1" r:id="rId1"/>
     <sheet name="@Types" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t>Id</t>
   </si>
@@ -27,7 +27,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Verdana"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>M</t>
     </r>
@@ -35,7 +35,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Verdana"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>odel</t>
     </r>
@@ -60,7 +60,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Verdana"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>T</t>
     </r>
@@ -68,7 +68,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Verdana"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>ank</t>
     </r>
@@ -87,7 +87,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Verdana"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>M</t>
     </r>
@@ -95,7 +95,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Verdana"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>axStar</t>
     </r>
@@ -108,34 +108,16 @@
   </si>
   <si>
     <t>uint32</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
   <si>
     <r>
       <rPr>
         <sz val="12"/>
         <rFont val="Verdana"/>
-        <charset val="134"/>
-      </rPr>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <charset val="134"/>
-      </rPr>
-      <t>tring</t>
-    </r>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Verdana"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>u</t>
     </r>
@@ -143,7 +125,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Verdana"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>int32</t>
     </r>
@@ -200,197 +182,140 @@
     <t>星级套件属性(没有填0)</t>
   </si>
   <si>
-    <t>奔驰</t>
-  </si>
-  <si>
-    <t>smart</t>
-  </si>
-  <si>
     <t>carIconAltas_json.small_1</t>
   </si>
   <si>
     <t>carIconAltas_json.big_1</t>
   </si>
   <si>
-    <t>本田</t>
-  </si>
-  <si>
-    <t>思域</t>
-  </si>
-  <si>
     <t>carIconAltas_json.small_2</t>
   </si>
   <si>
     <t>carIconAltas_json.big_2</t>
   </si>
   <si>
-    <t>大众</t>
-  </si>
-  <si>
-    <t>polo</t>
-  </si>
-  <si>
     <t>carIconAltas_json.small_3</t>
   </si>
   <si>
     <t>carIconAltas_json.big_3</t>
   </si>
   <si>
-    <t>丰田</t>
-  </si>
-  <si>
-    <t>汉兰达</t>
-  </si>
-  <si>
     <t>carIconAltas_json.small_4</t>
   </si>
   <si>
     <t>carIconAltas_json.big_4</t>
   </si>
   <si>
-    <t>奥迪</t>
-  </si>
-  <si>
-    <t>A4L</t>
-  </si>
-  <si>
     <t>carIconAltas_json.small_5</t>
   </si>
   <si>
     <t>carIconAltas_json.big_5</t>
   </si>
   <si>
-    <t>宝马</t>
-  </si>
-  <si>
-    <t>mini</t>
-  </si>
-  <si>
     <t>carIconAltas_json.small_6</t>
   </si>
   <si>
     <t>carIconAltas_json.big_6</t>
   </si>
   <si>
-    <t>雪佛莱</t>
-  </si>
-  <si>
-    <t>科迈罗</t>
-  </si>
-  <si>
     <t>carIconAltas_json.small_7</t>
   </si>
   <si>
     <t>carIconAltas_json.big_7</t>
   </si>
   <si>
-    <t>保时捷</t>
-  </si>
-  <si>
     <t>carIconAltas_json.small_8</t>
   </si>
   <si>
     <t>carIconAltas_json.big_8</t>
   </si>
   <si>
+    <t>carIconAltas_json.small_9</t>
+  </si>
+  <si>
+    <t>carIconAltas_json.big_9</t>
+  </si>
+  <si>
+    <t>carIconAltas_json.small_10</t>
+  </si>
+  <si>
+    <t>carIconAltas_json.big_10</t>
+  </si>
+  <si>
+    <t>TableName: "TCar" Package: "table" CSClassHeader: "[System.Serializable]"</t>
+  </si>
+  <si>
+    <t>ObjectType</t>
+  </si>
+  <si>
+    <t>FieldName</t>
+  </si>
+  <si>
+    <t>FieldType</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Meta</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>对象类型</t>
+  </si>
+  <si>
+    <t>字段名</t>
+  </si>
+  <si>
+    <t>字段类型</t>
+  </si>
+  <si>
+    <t>枚举值</t>
+  </si>
+  <si>
+    <t>别名</t>
+  </si>
+  <si>
+    <t>默认值</t>
+  </si>
+  <si>
+    <t>特性</t>
+  </si>
+  <si>
+    <t>注释</t>
+  </si>
+  <si>
+    <t>uint32</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>u</t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
         <rFont val="Verdana"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
-      <t>G</t>
+      <t>int32</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>级</t>
-    </r>
-  </si>
-  <si>
-    <t>carIconAltas_json.small_9</t>
-  </si>
-  <si>
-    <t>carIconAltas_json.big_9</t>
-  </si>
-  <si>
-    <t>劳斯劳斯</t>
-  </si>
-  <si>
-    <t>古斯特</t>
-  </si>
-  <si>
-    <t>carIconAltas_json.small_10</t>
-  </si>
-  <si>
-    <t>carIconAltas_json.big_10</t>
-  </si>
-  <si>
-    <t>TableName: "TCar" Package: "table" CSClassHeader: "[System.Serializable]"</t>
-  </si>
-  <si>
-    <t>ObjectType</t>
-  </si>
-  <si>
-    <t>FieldName</t>
-  </si>
-  <si>
-    <t>FieldType</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Alias</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>Meta</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>对象类型</t>
-  </si>
-  <si>
-    <t>字段名</t>
-  </si>
-  <si>
-    <t>字段类型</t>
-  </si>
-  <si>
-    <t>枚举值</t>
-  </si>
-  <si>
-    <t>别名</t>
-  </si>
-  <si>
-    <t>默认值</t>
-  </si>
-  <si>
-    <t>特性</t>
-  </si>
-  <si>
-    <t>注释</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -399,7 +324,7 @@
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -412,158 +337,12 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -576,194 +355,8 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -771,266 +364,24 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="49" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1050,62 +401,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
-    <cellStyle name="常规 2" xfId="49"/>
+    <cellStyle name="常规 2" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1431,28 +732,28 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="6.6" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.9" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.6" customWidth="1"/>
-    <col min="6" max="6" width="23.9" customWidth="1"/>
-    <col min="7" max="7" width="24.4" customWidth="1"/>
-    <col min="12" max="12" width="7.4" customWidth="1"/>
-    <col min="14" max="14" width="18.7" customWidth="1"/>
+    <col min="2" max="2" width="6.59765625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.8984375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.59765625" customWidth="1"/>
+    <col min="6" max="6" width="23.8984375" customWidth="1"/>
+    <col min="7" max="7" width="24.3984375" customWidth="1"/>
+    <col min="12" max="12" width="7.3984375" customWidth="1"/>
+    <col min="14" max="14" width="18.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -1508,30 +809,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>17</v>
+      <c r="B2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>15</v>
@@ -1554,81 +855,81 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5">
         <v>1001</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>37</v>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H5">
         <v>1001</v>
@@ -1665,21 +966,21 @@
       <c r="A6">
         <v>1002</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>41</v>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10">
+        <v>1</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H6">
         <v>1002</v>
@@ -1716,21 +1017,21 @@
       <c r="A7">
         <v>1003</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>45</v>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H7">
         <v>1003</v>
@@ -1767,21 +1068,21 @@
       <c r="A8">
         <v>1004</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>49</v>
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10">
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H8">
         <v>1004</v>
@@ -1818,21 +1119,21 @@
       <c r="A9">
         <v>1005</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>53</v>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H9">
         <v>1005</v>
@@ -1869,21 +1170,21 @@
       <c r="A10">
         <v>1006</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>57</v>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10">
+        <v>1</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="H10">
         <v>1006</v>
@@ -1920,21 +1221,21 @@
       <c r="A11">
         <v>1007</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>61</v>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10">
+        <v>1</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="H11">
         <v>1007</v>
@@ -1971,21 +1272,21 @@
       <c r="A12">
         <v>1008</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="11">
-        <v>911</v>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="H12">
         <v>1008</v>
@@ -2022,21 +1323,21 @@
       <c r="A13">
         <v>1009</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>67</v>
+      <c r="B13" s="9">
+        <v>1</v>
+      </c>
+      <c r="C13" s="10">
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="H13">
         <v>1009</v>
@@ -2073,21 +1374,21 @@
       <c r="A14">
         <v>1010</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>71</v>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10">
+        <v>1</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="H14">
         <v>1010</v>
@@ -2120,15 +1421,16 @@
         <v>420</v>
       </c>
     </row>
-    <row r="15" spans="5:5">
+    <row r="15" spans="1:17">
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="5:5">
+    <row r="16" spans="1:17">
       <c r="E16" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2137,80 +1439,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="83.5" style="1" customWidth="1"/>
-    <col min="2" max="8" width="8.8" style="1"/>
-    <col min="9" max="16384" width="8.8" style="2"/>
+    <col min="2" max="8" width="8.796875" style="1"/>
+    <col min="9" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>

</xml_diff>